<commit_message>
Correzione errori come da richiesta
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.0/report-checklist.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insiel.sharepoint.com/sites/O365-Clinico/Documenti condivisi/PNRR-FSE- Indicatori e  CDA2-Clinico Cardiologia SEI/Clinico/Accreditamento/Documenti da spedire/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\accreditamento\Accreditamento CLINICO\S1#060000000000XX\INSIEL\CLINICO\G4.3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:1_{4912A481-5CF5-4C12-BC3C-8C60613AB0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C57C4598-D13C-4CDD-AFAF-52BC9A5FE0B8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7276E4B-CCD1-4269-8900-6E69C59C7A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="397">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -377,9 +377,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.60.4.4.196994261359e62f2e1c811dda37b940b1a01e6e554824be25e92936673e5076.e5dd0ea25b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>l'APPLICATIVO NON PREVEDE QUESTO CASO</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT2</t>
@@ -1642,6 +1639,13 @@
   </si>
   <si>
     <t>35,43,51,122,123,124,125,126,127,128,129,130,131,132,133,134,135,136,137,138,139,140,141,142,143,144,145,146</t>
+  </si>
+  <si>
+    <t>test non eseguibile perchè sarà oggetto dell'accreditamento del middleware regionale</t>
+  </si>
+  <si>
+    <t>"status": 504,
+"detail": la richiesta al gateway è andata in timeout</t>
   </si>
 </sst>
 </file>
@@ -2193,25 +2197,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3581,11 +3585,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B93" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3618,14 +3622,14 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="18.75">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -3638,14 +3642,14 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="50"/>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="47"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -3660,10 +3664,10 @@
     <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="51"/>
       <c r="B4" s="52"/>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -3679,10 +3683,10 @@
     <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="53"/>
       <c r="B5" s="54"/>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="47"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -3696,7 +3700,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="44"/>
-      <c r="B6" s="55"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4085,9 +4089,7 @@
       <c r="L19" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="37" t="s">
-        <v>65</v>
-      </c>
+      <c r="M19" s="37"/>
       <c r="N19" s="20"/>
       <c r="O19" s="21"/>
     </row>
@@ -4102,10 +4104,10 @@
         <v>58</v>
       </c>
       <c r="D20" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>66</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>67</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="18"/>
@@ -4133,10 +4135,10 @@
         <v>58</v>
       </c>
       <c r="D21" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>69</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="18"/>
@@ -4164,10 +4166,10 @@
         <v>58</v>
       </c>
       <c r="D22" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="18"/>
@@ -4192,13 +4194,13 @@
         <v>29</v>
       </c>
       <c r="C23" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="E23" s="16" t="s">
         <v>73</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>74</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="18"/>
@@ -4219,13 +4221,13 @@
         <v>29</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>76</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="18"/>
@@ -4246,13 +4248,13 @@
         <v>29</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D25" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>78</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
@@ -4273,13 +4275,13 @@
         <v>29</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
@@ -4300,13 +4302,13 @@
         <v>29</v>
       </c>
       <c r="C27" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="E27" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>83</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -4327,13 +4329,13 @@
         <v>29</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>84</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>85</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -4354,13 +4356,13 @@
         <v>29</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>87</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
@@ -4381,13 +4383,13 @@
         <v>29</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>89</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
@@ -4408,13 +4410,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="E31" s="16" t="s">
         <v>91</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>92</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
@@ -4435,13 +4437,13 @@
         <v>29</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>93</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>94</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
@@ -4462,13 +4464,13 @@
         <v>29</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
@@ -4489,13 +4491,13 @@
         <v>29</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>98</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -4519,10 +4521,10 @@
         <v>30</v>
       </c>
       <c r="D35" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>100</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
@@ -4548,19 +4550,23 @@
         <v>41</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
       <c r="I36" s="18"/>
       <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
+      <c r="K36" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
+      <c r="M36" s="19" t="s">
+        <v>395</v>
+      </c>
       <c r="N36" s="20" t="s">
         <v>48</v>
       </c>
@@ -4577,19 +4583,23 @@
         <v>58</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
       <c r="I37" s="18"/>
       <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
+      <c r="K37" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
+      <c r="M37" s="19" t="s">
+        <v>395</v>
+      </c>
       <c r="N37" s="20" t="s">
         <v>48</v>
       </c>
@@ -4603,13 +4613,13 @@
         <v>29</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
@@ -4632,13 +4642,13 @@
         <v>29</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
@@ -4661,13 +4671,13 @@
         <v>29</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
@@ -4693,10 +4703,10 @@
         <v>30</v>
       </c>
       <c r="D41" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" s="16" t="s">
         <v>106</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>107</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
@@ -4722,19 +4732,23 @@
         <v>41</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
       <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
+      <c r="K42" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
+      <c r="M42" s="19" t="s">
+        <v>395</v>
+      </c>
       <c r="N42" s="20" t="s">
         <v>48</v>
       </c>
@@ -4751,19 +4765,23 @@
         <v>58</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
       <c r="I43" s="18"/>
       <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
+      <c r="K43" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
+      <c r="M43" s="19" t="s">
+        <v>395</v>
+      </c>
       <c r="N43" s="20" t="s">
         <v>48</v>
       </c>
@@ -4777,13 +4795,13 @@
         <v>29</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
@@ -4806,13 +4824,13 @@
         <v>29</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
@@ -4835,13 +4853,13 @@
         <v>29</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
@@ -4867,10 +4885,10 @@
         <v>30</v>
       </c>
       <c r="D47" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="16" t="s">
         <v>113</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>114</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
@@ -4896,18 +4914,24 @@
         <v>41</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
       <c r="I48" s="18"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
+      <c r="J48" s="37" t="s">
+        <v>396</v>
+      </c>
+      <c r="K48" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="L48" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="M48" s="19"/>
       <c r="N48" s="20" t="s">
         <v>48</v>
@@ -4925,18 +4949,24 @@
         <v>58</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="18"/>
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
-      <c r="J49" s="19"/>
-      <c r="K49" s="19"/>
-      <c r="L49" s="19"/>
+      <c r="J49" s="37" t="s">
+        <v>396</v>
+      </c>
+      <c r="K49" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="L49" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="M49" s="19"/>
       <c r="N49" s="20" t="s">
         <v>48</v>
@@ -4951,13 +4981,13 @@
         <v>29</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F50" s="17"/>
       <c r="G50" s="18"/>
@@ -4980,13 +5010,13 @@
         <v>29</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="18"/>
@@ -5009,13 +5039,13 @@
         <v>29</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="18"/>
@@ -5041,10 +5071,10 @@
         <v>30</v>
       </c>
       <c r="D53" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="18"/>
@@ -5070,10 +5100,10 @@
         <v>30</v>
       </c>
       <c r="D54" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>123</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="18"/>
@@ -5099,10 +5129,10 @@
         <v>30</v>
       </c>
       <c r="D55" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E55" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>125</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="18"/>
@@ -5128,10 +5158,10 @@
         <v>30</v>
       </c>
       <c r="D56" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="18"/>
@@ -5157,10 +5187,10 @@
         <v>30</v>
       </c>
       <c r="D57" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E57" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>129</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="18"/>
@@ -5186,10 +5216,10 @@
         <v>30</v>
       </c>
       <c r="D58" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E58" s="16" t="s">
         <v>130</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>131</v>
       </c>
       <c r="F58" s="17"/>
       <c r="G58" s="18"/>
@@ -5215,10 +5245,10 @@
         <v>30</v>
       </c>
       <c r="D59" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>133</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="18"/>
@@ -5244,10 +5274,10 @@
         <v>30</v>
       </c>
       <c r="D60" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E60" s="16" t="s">
         <v>134</v>
-      </c>
-      <c r="E60" s="16" t="s">
-        <v>135</v>
       </c>
       <c r="F60" s="17"/>
       <c r="G60" s="18"/>
@@ -5273,10 +5303,10 @@
         <v>30</v>
       </c>
       <c r="D61" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E61" s="16" t="s">
         <v>136</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>137</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="18"/>
@@ -5302,10 +5332,10 @@
         <v>30</v>
       </c>
       <c r="D62" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" s="16" t="s">
         <v>138</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>139</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="18"/>
@@ -5331,10 +5361,10 @@
         <v>30</v>
       </c>
       <c r="D63" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E63" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="18"/>
@@ -5360,10 +5390,10 @@
         <v>41</v>
       </c>
       <c r="D64" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E64" s="16" t="s">
         <v>142</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>143</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="18"/>
@@ -5375,7 +5405,7 @@
       </c>
       <c r="L64" s="19"/>
       <c r="M64" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N64" s="20"/>
       <c r="O64" s="21"/>
@@ -5391,31 +5421,31 @@
         <v>41</v>
       </c>
       <c r="D65" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E65" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="F65" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="F65" s="17" t="s">
+      <c r="G65" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="G65" s="18" t="s">
+      <c r="H65" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="H65" s="18" t="s">
+      <c r="I65" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="I65" s="18" t="s">
+      <c r="J65" s="37" t="s">
         <v>150</v>
-      </c>
-      <c r="J65" s="19" t="s">
-        <v>151</v>
       </c>
       <c r="K65" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L65" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M65" s="19"/>
       <c r="N65" s="20" t="s">
@@ -5434,31 +5464,31 @@
         <v>41</v>
       </c>
       <c r="D66" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E66" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="F66" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="F66" s="17" t="s">
+      <c r="G66" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G66" s="18" t="s">
+      <c r="H66" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="H66" s="18" t="s">
+      <c r="I66" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="I66" s="18" t="s">
+      <c r="J66" s="19" t="s">
         <v>158</v>
-      </c>
-      <c r="J66" s="19" t="s">
-        <v>159</v>
       </c>
       <c r="K66" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L66" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N66" s="20" t="s">
         <v>48</v>
@@ -5476,10 +5506,10 @@
         <v>41</v>
       </c>
       <c r="D67" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E67" s="16" t="s">
         <v>160</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>161</v>
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="18"/>
@@ -5509,31 +5539,31 @@
         <v>41</v>
       </c>
       <c r="D68" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E68" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="F68" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="F68" s="17" t="s">
+      <c r="G68" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G68" s="18" t="s">
+      <c r="H68" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="H68" s="18" t="s">
+      <c r="I68" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="I68" s="18" t="s">
+      <c r="J68" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="J68" s="19" t="s">
-        <v>168</v>
       </c>
       <c r="K68" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L68" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M68" s="19"/>
       <c r="N68" s="20" t="s">
@@ -5552,31 +5582,31 @@
         <v>41</v>
       </c>
       <c r="D69" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E69" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="F69" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="F69" s="17" t="s">
+      <c r="G69" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="G69" s="18" t="s">
+      <c r="H69" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="H69" s="18" t="s">
+      <c r="I69" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="I69" s="18" t="s">
+      <c r="J69" s="19" t="s">
         <v>174</v>
-      </c>
-      <c r="J69" s="19" t="s">
-        <v>175</v>
       </c>
       <c r="K69" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L69" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M69" s="19"/>
       <c r="N69" s="20" t="s">
@@ -5595,31 +5625,31 @@
         <v>41</v>
       </c>
       <c r="D70" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E70" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="F70" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="F70" s="17" t="s">
+      <c r="G70" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="G70" s="18" t="s">
+      <c r="H70" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="H70" s="39" t="s">
+      <c r="I70" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="I70" s="39" t="s">
+      <c r="J70" s="37" t="s">
         <v>181</v>
-      </c>
-      <c r="J70" s="37" t="s">
-        <v>182</v>
       </c>
       <c r="K70" s="37" t="s">
         <v>48</v>
       </c>
       <c r="L70" s="37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M70" s="19"/>
       <c r="N70" s="20" t="s">
@@ -5638,31 +5668,31 @@
         <v>41</v>
       </c>
       <c r="D71" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E71" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="F71" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="F71" s="17" t="s">
+      <c r="G71" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="G71" s="18" t="s">
+      <c r="H71" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="H71" s="39" t="s">
+      <c r="I71" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="I71" s="18" t="s">
+      <c r="J71" s="19" t="s">
         <v>188</v>
-      </c>
-      <c r="J71" s="19" t="s">
-        <v>189</v>
       </c>
       <c r="K71" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L71" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M71" s="19"/>
       <c r="N71" s="20" t="s">
@@ -5681,10 +5711,10 @@
         <v>41</v>
       </c>
       <c r="D72" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E72" s="16" t="s">
         <v>190</v>
-      </c>
-      <c r="E72" s="16" t="s">
-        <v>191</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="18"/>
@@ -5714,10 +5744,10 @@
         <v>41</v>
       </c>
       <c r="D73" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E73" s="16" t="s">
         <v>192</v>
-      </c>
-      <c r="E73" s="16" t="s">
-        <v>193</v>
       </c>
       <c r="F73" s="17"/>
       <c r="G73" s="18"/>
@@ -5747,10 +5777,10 @@
         <v>41</v>
       </c>
       <c r="D74" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E74" s="16" t="s">
         <v>194</v>
-      </c>
-      <c r="E74" s="16" t="s">
-        <v>195</v>
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="18"/>
@@ -5769,7 +5799,7 @@
       </c>
       <c r="O74" s="21"/>
     </row>
-    <row r="75" spans="1:15" ht="120">
+    <row r="75" spans="1:15" ht="120.75" thickBot="1">
       <c r="A75" s="14">
         <v>74</v>
       </c>
@@ -5780,10 +5810,10 @@
         <v>41</v>
       </c>
       <c r="D75" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E75" s="16" t="s">
         <v>196</v>
-      </c>
-      <c r="E75" s="16" t="s">
-        <v>197</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="18"/>
@@ -5802,7 +5832,7 @@
       </c>
       <c r="O75" s="21"/>
     </row>
-    <row r="76" spans="1:15" ht="135">
+    <row r="76" spans="1:15" ht="135.75" thickBot="1">
       <c r="A76" s="14">
         <v>75</v>
       </c>
@@ -5813,10 +5843,10 @@
         <v>58</v>
       </c>
       <c r="D76" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E76" s="16" t="s">
         <v>198</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>199</v>
       </c>
       <c r="F76" s="17"/>
       <c r="G76" s="18"/>
@@ -5828,14 +5858,14 @@
       </c>
       <c r="L76" s="19"/>
       <c r="M76" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N76" s="20" t="s">
         <v>48</v>
       </c>
       <c r="O76" s="21"/>
     </row>
-    <row r="77" spans="1:15" ht="180">
+    <row r="77" spans="1:15" ht="180.75" thickBot="1">
       <c r="A77" s="14">
         <v>76</v>
       </c>
@@ -5846,31 +5876,31 @@
         <v>58</v>
       </c>
       <c r="D77" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="E77" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="F77" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="F77" s="17" t="s">
+      <c r="G77" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="G77" s="18" t="s">
+      <c r="H77" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H77" s="18" t="s">
+      <c r="I77" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="I77" s="18" t="s">
+      <c r="J77" s="19" t="s">
         <v>205</v>
-      </c>
-      <c r="J77" s="19" t="s">
-        <v>206</v>
       </c>
       <c r="K77" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L77" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M77" s="19"/>
       <c r="N77" s="20" t="s">
@@ -5878,7 +5908,7 @@
       </c>
       <c r="O77" s="21"/>
     </row>
-    <row r="78" spans="1:15" ht="225">
+    <row r="78" spans="1:15" ht="225.75" thickBot="1">
       <c r="A78" s="14">
         <v>77</v>
       </c>
@@ -5889,31 +5919,31 @@
         <v>58</v>
       </c>
       <c r="D78" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E78" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="E78" s="16" t="s">
+      <c r="F78" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="F78" s="17" t="s">
+      <c r="G78" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="G78" s="18" t="s">
+      <c r="H78" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="H78" s="18" t="s">
+      <c r="I78" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="I78" s="18" t="s">
+      <c r="J78" s="19" t="s">
         <v>212</v>
-      </c>
-      <c r="J78" s="19" t="s">
-        <v>213</v>
       </c>
       <c r="K78" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L78" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M78" s="19"/>
       <c r="N78" s="20" t="s">
@@ -5921,7 +5951,7 @@
       </c>
       <c r="O78" s="21"/>
     </row>
-    <row r="79" spans="1:15" ht="105">
+    <row r="79" spans="1:15" ht="105.75" thickBot="1">
       <c r="A79" s="14">
         <v>78</v>
       </c>
@@ -5932,10 +5962,10 @@
         <v>58</v>
       </c>
       <c r="D79" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E79" s="16" t="s">
         <v>214</v>
-      </c>
-      <c r="E79" s="16" t="s">
-        <v>215</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="18"/>
@@ -5954,7 +5984,7 @@
       </c>
       <c r="O79" s="21"/>
     </row>
-    <row r="80" spans="1:15" ht="225">
+    <row r="80" spans="1:15" ht="225.75" thickBot="1">
       <c r="A80" s="14">
         <v>79</v>
       </c>
@@ -5965,31 +5995,31 @@
         <v>58</v>
       </c>
       <c r="D80" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="E80" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="E80" s="16" t="s">
+      <c r="F80" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="F80" s="17" t="s">
+      <c r="G80" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="G80" s="18" t="s">
+      <c r="H80" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="H80" s="18" t="s">
+      <c r="I80" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="I80" s="39" t="s">
-        <v>221</v>
-      </c>
       <c r="J80" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K80" s="37" t="s">
         <v>48</v>
       </c>
       <c r="L80" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M80" s="19"/>
       <c r="N80" s="20" t="s">
@@ -5997,7 +6027,7 @@
       </c>
       <c r="O80" s="21"/>
     </row>
-    <row r="81" spans="1:15" ht="120">
+    <row r="81" spans="1:15" ht="120.75" thickBot="1">
       <c r="A81" s="14">
         <v>80</v>
       </c>
@@ -6008,31 +6038,31 @@
         <v>58</v>
       </c>
       <c r="D81" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E81" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="E81" s="16" t="s">
+      <c r="F81" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="F81" s="17" t="s">
+      <c r="G81" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="G81" s="39" t="s">
+      <c r="H81" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="H81" s="39" t="s">
+      <c r="I81" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="I81" s="39" t="s">
+      <c r="J81" s="37" t="s">
         <v>227</v>
-      </c>
-      <c r="J81" s="37" t="s">
-        <v>228</v>
       </c>
       <c r="K81" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L81" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M81" s="19"/>
       <c r="N81" s="20" t="s">
@@ -6040,7 +6070,7 @@
       </c>
       <c r="O81" s="21"/>
     </row>
-    <row r="82" spans="1:15" ht="120">
+    <row r="82" spans="1:15" ht="120.75" thickBot="1">
       <c r="A82" s="14">
         <v>81</v>
       </c>
@@ -6051,10 +6081,10 @@
         <v>58</v>
       </c>
       <c r="D82" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="E82" s="16" t="s">
         <v>229</v>
-      </c>
-      <c r="E82" s="16" t="s">
-        <v>230</v>
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="18"/>
@@ -6073,7 +6103,7 @@
       </c>
       <c r="O82" s="21"/>
     </row>
-    <row r="83" spans="1:15" ht="315">
+    <row r="83" spans="1:15" ht="315.75" thickBot="1">
       <c r="A83" s="14">
         <v>82</v>
       </c>
@@ -6084,31 +6114,31 @@
         <v>58</v>
       </c>
       <c r="D83" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E83" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="F83" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="F83" s="17" t="s">
+      <c r="G83" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="G83" s="39" t="s">
+      <c r="H83" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="H83" s="39" t="s">
+      <c r="I83" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="I83" s="39" t="s">
+      <c r="J83" s="37" t="s">
         <v>236</v>
-      </c>
-      <c r="J83" s="37" t="s">
-        <v>237</v>
       </c>
       <c r="K83" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L83" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M83" s="19"/>
       <c r="N83" s="20" t="s">
@@ -6116,7 +6146,7 @@
       </c>
       <c r="O83" s="21"/>
     </row>
-    <row r="84" spans="1:15" ht="225">
+    <row r="84" spans="1:15" ht="225.75" thickBot="1">
       <c r="A84" s="14">
         <v>83</v>
       </c>
@@ -6127,31 +6157,31 @@
         <v>58</v>
       </c>
       <c r="D84" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="E84" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="F84" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="F84" s="38" t="s">
+      <c r="G84" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="G84" s="39" t="s">
+      <c r="H84" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="H84" s="39" t="s">
+      <c r="I84" s="39" t="s">
         <v>242</v>
       </c>
-      <c r="I84" s="39" t="s">
+      <c r="J84" s="37" t="s">
         <v>243</v>
-      </c>
-      <c r="J84" s="37" t="s">
-        <v>244</v>
       </c>
       <c r="K84" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L84" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M84" s="19"/>
       <c r="N84" s="20" t="s">
@@ -6159,7 +6189,7 @@
       </c>
       <c r="O84" s="21"/>
     </row>
-    <row r="85" spans="1:15" ht="135">
+    <row r="85" spans="1:15" ht="135.75" thickBot="1">
       <c r="A85" s="14">
         <v>84</v>
       </c>
@@ -6170,31 +6200,31 @@
         <v>58</v>
       </c>
       <c r="D85" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E85" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="E85" s="16" t="s">
+      <c r="F85" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="F85" s="38" t="s">
+      <c r="G85" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="G85" s="39" t="s">
+      <c r="H85" s="39" t="s">
         <v>248</v>
       </c>
-      <c r="H85" s="39" t="s">
+      <c r="I85" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="I85" s="39" t="s">
+      <c r="J85" s="37" t="s">
         <v>250</v>
-      </c>
-      <c r="J85" s="37" t="s">
-        <v>251</v>
       </c>
       <c r="K85" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L85" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M85" s="19"/>
       <c r="N85" s="20" t="s">
@@ -6202,7 +6232,7 @@
       </c>
       <c r="O85" s="21"/>
     </row>
-    <row r="86" spans="1:15" ht="210">
+    <row r="86" spans="1:15" ht="210.75" thickBot="1">
       <c r="A86" s="14">
         <v>85</v>
       </c>
@@ -6213,31 +6243,31 @@
         <v>58</v>
       </c>
       <c r="D86" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E86" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="E86" s="43" t="s">
+      <c r="F86" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="F86" s="38" t="s">
+      <c r="G86" s="39" t="s">
         <v>254</v>
       </c>
-      <c r="G86" s="39" t="s">
+      <c r="H86" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="H86" s="39" t="s">
+      <c r="I86" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="I86" s="39" t="s">
+      <c r="J86" s="37" t="s">
         <v>257</v>
-      </c>
-      <c r="J86" s="37" t="s">
-        <v>258</v>
       </c>
       <c r="K86" s="19" t="s">
         <v>48</v>
       </c>
       <c r="L86" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M86" s="19"/>
       <c r="N86" s="20" t="s">
@@ -6245,7 +6275,7 @@
       </c>
       <c r="O86" s="21"/>
     </row>
-    <row r="87" spans="1:15" ht="120">
+    <row r="87" spans="1:15" ht="120.75" thickBot="1">
       <c r="A87" s="14">
         <v>86</v>
       </c>
@@ -6256,10 +6286,10 @@
         <v>58</v>
       </c>
       <c r="D87" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="E87" s="16" t="s">
         <v>259</v>
-      </c>
-      <c r="E87" s="16" t="s">
-        <v>260</v>
       </c>
       <c r="F87" s="17"/>
       <c r="G87" s="18"/>
@@ -6278,7 +6308,7 @@
       </c>
       <c r="O87" s="21"/>
     </row>
-    <row r="88" spans="1:15" ht="135">
+    <row r="88" spans="1:15" ht="135.75" thickBot="1">
       <c r="A88" s="14">
         <v>87</v>
       </c>
@@ -6289,10 +6319,10 @@
         <v>58</v>
       </c>
       <c r="D88" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="E88" s="16" t="s">
         <v>261</v>
-      </c>
-      <c r="E88" s="16" t="s">
-        <v>262</v>
       </c>
       <c r="F88" s="17"/>
       <c r="G88" s="18"/>
@@ -6311,7 +6341,7 @@
       </c>
       <c r="O88" s="21"/>
     </row>
-    <row r="89" spans="1:15" ht="120">
+    <row r="89" spans="1:15" ht="120.75" thickBot="1">
       <c r="A89" s="14">
         <v>88</v>
       </c>
@@ -6322,10 +6352,10 @@
         <v>58</v>
       </c>
       <c r="D89" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E89" s="16" t="s">
         <v>263</v>
-      </c>
-      <c r="E89" s="16" t="s">
-        <v>264</v>
       </c>
       <c r="F89" s="17"/>
       <c r="G89" s="18"/>
@@ -6344,7 +6374,7 @@
       </c>
       <c r="O89" s="21"/>
     </row>
-    <row r="90" spans="1:15" ht="105">
+    <row r="90" spans="1:15" ht="105.75" thickBot="1">
       <c r="A90" s="14">
         <v>89</v>
       </c>
@@ -6355,10 +6385,10 @@
         <v>58</v>
       </c>
       <c r="D90" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="E90" s="16" t="s">
         <v>265</v>
-      </c>
-      <c r="E90" s="16" t="s">
-        <v>266</v>
       </c>
       <c r="F90" s="17"/>
       <c r="G90" s="18"/>
@@ -6377,7 +6407,7 @@
       </c>
       <c r="O90" s="21"/>
     </row>
-    <row r="91" spans="1:15" ht="105">
+    <row r="91" spans="1:15" ht="105.75" thickBot="1">
       <c r="A91" s="14">
         <v>90</v>
       </c>
@@ -6388,10 +6418,10 @@
         <v>58</v>
       </c>
       <c r="D91" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="E91" s="16" t="s">
         <v>267</v>
-      </c>
-      <c r="E91" s="16" t="s">
-        <v>268</v>
       </c>
       <c r="F91" s="17"/>
       <c r="G91" s="18"/>
@@ -6410,7 +6440,7 @@
       </c>
       <c r="O91" s="21"/>
     </row>
-    <row r="92" spans="1:15" ht="120">
+    <row r="92" spans="1:15" ht="120.75" thickBot="1">
       <c r="A92" s="14">
         <v>91</v>
       </c>
@@ -6421,10 +6451,10 @@
         <v>58</v>
       </c>
       <c r="D92" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="E92" s="16" t="s">
         <v>269</v>
-      </c>
-      <c r="E92" s="16" t="s">
-        <v>270</v>
       </c>
       <c r="F92" s="17"/>
       <c r="G92" s="18"/>
@@ -6443,7 +6473,7 @@
       </c>
       <c r="O92" s="21"/>
     </row>
-    <row r="93" spans="1:15" ht="120">
+    <row r="93" spans="1:15" ht="120.75" thickBot="1">
       <c r="A93" s="14">
         <v>92</v>
       </c>
@@ -6454,10 +6484,10 @@
         <v>58</v>
       </c>
       <c r="D93" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="E93" s="16" t="s">
         <v>271</v>
-      </c>
-      <c r="E93" s="16" t="s">
-        <v>272</v>
       </c>
       <c r="F93" s="17"/>
       <c r="G93" s="18"/>
@@ -6487,10 +6517,10 @@
         <v>58</v>
       </c>
       <c r="D94" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="E94" s="16" t="s">
         <v>273</v>
-      </c>
-      <c r="E94" s="16" t="s">
-        <v>274</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="18"/>
@@ -6517,13 +6547,13 @@
         <v>29</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D95" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="E95" s="16" t="s">
         <v>275</v>
-      </c>
-      <c r="E95" s="16" t="s">
-        <v>276</v>
       </c>
       <c r="F95" s="17"/>
       <c r="G95" s="18"/>
@@ -6546,13 +6576,13 @@
         <v>29</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D96" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="E96" s="16" t="s">
         <v>277</v>
-      </c>
-      <c r="E96" s="16" t="s">
-        <v>278</v>
       </c>
       <c r="F96" s="17"/>
       <c r="G96" s="18"/>
@@ -6575,13 +6605,13 @@
         <v>29</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D97" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="E97" s="16" t="s">
         <v>279</v>
-      </c>
-      <c r="E97" s="16" t="s">
-        <v>280</v>
       </c>
       <c r="F97" s="17"/>
       <c r="G97" s="18"/>
@@ -6604,13 +6634,13 @@
         <v>29</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D98" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="E98" s="16" t="s">
         <v>281</v>
-      </c>
-      <c r="E98" s="16" t="s">
-        <v>282</v>
       </c>
       <c r="F98" s="17"/>
       <c r="G98" s="18"/>
@@ -6633,13 +6663,13 @@
         <v>29</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D99" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="E99" s="16" t="s">
         <v>283</v>
-      </c>
-      <c r="E99" s="16" t="s">
-        <v>284</v>
       </c>
       <c r="F99" s="17"/>
       <c r="G99" s="18"/>
@@ -6662,13 +6692,13 @@
         <v>29</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D100" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="E100" s="16" t="s">
         <v>285</v>
-      </c>
-      <c r="E100" s="16" t="s">
-        <v>286</v>
       </c>
       <c r="F100" s="17"/>
       <c r="G100" s="18"/>
@@ -6691,13 +6721,13 @@
         <v>29</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D101" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="E101" s="16" t="s">
         <v>287</v>
-      </c>
-      <c r="E101" s="16" t="s">
-        <v>288</v>
       </c>
       <c r="F101" s="17"/>
       <c r="G101" s="18"/>
@@ -6720,13 +6750,13 @@
         <v>29</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D102" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="E102" s="16" t="s">
         <v>289</v>
-      </c>
-      <c r="E102" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="F102" s="17"/>
       <c r="G102" s="18"/>
@@ -6749,13 +6779,13 @@
         <v>29</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D103" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="E103" s="16" t="s">
         <v>291</v>
-      </c>
-      <c r="E103" s="16" t="s">
-        <v>292</v>
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="18"/>
@@ -6778,13 +6808,13 @@
         <v>29</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D104" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="E104" s="16" t="s">
         <v>293</v>
-      </c>
-      <c r="E104" s="16" t="s">
-        <v>294</v>
       </c>
       <c r="F104" s="17"/>
       <c r="G104" s="18"/>
@@ -6807,13 +6837,13 @@
         <v>29</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D105" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="E105" s="16" t="s">
         <v>295</v>
-      </c>
-      <c r="E105" s="16" t="s">
-        <v>296</v>
       </c>
       <c r="F105" s="17"/>
       <c r="G105" s="18"/>
@@ -6836,13 +6866,13 @@
         <v>29</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D106" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="E106" s="16" t="s">
         <v>297</v>
-      </c>
-      <c r="E106" s="16" t="s">
-        <v>298</v>
       </c>
       <c r="F106" s="17"/>
       <c r="G106" s="18"/>
@@ -6865,13 +6895,13 @@
         <v>29</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D107" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="E107" s="16" t="s">
         <v>299</v>
-      </c>
-      <c r="E107" s="16" t="s">
-        <v>300</v>
       </c>
       <c r="F107" s="17"/>
       <c r="G107" s="18"/>
@@ -6894,13 +6924,13 @@
         <v>29</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D108" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="E108" s="16" t="s">
         <v>301</v>
-      </c>
-      <c r="E108" s="16" t="s">
-        <v>302</v>
       </c>
       <c r="F108" s="17"/>
       <c r="G108" s="18"/>
@@ -6923,13 +6953,13 @@
         <v>29</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D109" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="E109" s="16" t="s">
         <v>303</v>
-      </c>
-      <c r="E109" s="16" t="s">
-        <v>304</v>
       </c>
       <c r="F109" s="17"/>
       <c r="G109" s="18"/>
@@ -6952,13 +6982,13 @@
         <v>29</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D110" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="E110" s="16" t="s">
         <v>305</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>306</v>
       </c>
       <c r="F110" s="17"/>
       <c r="G110" s="18"/>
@@ -6981,13 +7011,13 @@
         <v>29</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D111" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="E111" s="16" t="s">
         <v>307</v>
-      </c>
-      <c r="E111" s="16" t="s">
-        <v>308</v>
       </c>
       <c r="F111" s="17"/>
       <c r="G111" s="18"/>
@@ -7010,13 +7040,13 @@
         <v>29</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D112" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="E112" s="16" t="s">
         <v>309</v>
-      </c>
-      <c r="E112" s="16" t="s">
-        <v>310</v>
       </c>
       <c r="F112" s="17"/>
       <c r="G112" s="18"/>
@@ -7039,13 +7069,13 @@
         <v>29</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D113" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="E113" s="16" t="s">
         <v>311</v>
-      </c>
-      <c r="E113" s="16" t="s">
-        <v>312</v>
       </c>
       <c r="F113" s="17"/>
       <c r="G113" s="18"/>
@@ -7068,13 +7098,13 @@
         <v>29</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D114" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="E114" s="16" t="s">
         <v>313</v>
-      </c>
-      <c r="E114" s="16" t="s">
-        <v>314</v>
       </c>
       <c r="F114" s="17"/>
       <c r="G114" s="18"/>
@@ -7097,13 +7127,13 @@
         <v>29</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D115" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="E115" s="16" t="s">
         <v>315</v>
-      </c>
-      <c r="E115" s="16" t="s">
-        <v>316</v>
       </c>
       <c r="F115" s="17"/>
       <c r="G115" s="18"/>
@@ -7126,13 +7156,13 @@
         <v>29</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D116" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E116" s="16" t="s">
         <v>317</v>
-      </c>
-      <c r="E116" s="16" t="s">
-        <v>318</v>
       </c>
       <c r="F116" s="17"/>
       <c r="G116" s="18"/>
@@ -7155,13 +7185,13 @@
         <v>29</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D117" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="E117" s="16" t="s">
         <v>319</v>
-      </c>
-      <c r="E117" s="16" t="s">
-        <v>320</v>
       </c>
       <c r="F117" s="17"/>
       <c r="G117" s="18"/>
@@ -7184,13 +7214,13 @@
         <v>29</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D118" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="E118" s="16" t="s">
         <v>321</v>
-      </c>
-      <c r="E118" s="16" t="s">
-        <v>322</v>
       </c>
       <c r="F118" s="17"/>
       <c r="G118" s="18"/>
@@ -7213,13 +7243,13 @@
         <v>29</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D119" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="E119" s="16" t="s">
         <v>323</v>
-      </c>
-      <c r="E119" s="16" t="s">
-        <v>324</v>
       </c>
       <c r="F119" s="17"/>
       <c r="G119" s="18"/>
@@ -7242,13 +7272,13 @@
         <v>29</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D120" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="E120" s="16" t="s">
         <v>325</v>
-      </c>
-      <c r="E120" s="16" t="s">
-        <v>326</v>
       </c>
       <c r="F120" s="17"/>
       <c r="G120" s="18"/>
@@ -7271,13 +7301,13 @@
         <v>29</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D121" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="E121" s="16" t="s">
         <v>327</v>
-      </c>
-      <c r="E121" s="16" t="s">
-        <v>328</v>
       </c>
       <c r="F121" s="17"/>
       <c r="G121" s="18"/>
@@ -7300,13 +7330,13 @@
         <v>29</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D122" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="E122" s="16" t="s">
         <v>329</v>
-      </c>
-      <c r="E122" s="16" t="s">
-        <v>330</v>
       </c>
       <c r="F122" s="17"/>
       <c r="G122" s="18"/>
@@ -7329,13 +7359,13 @@
         <v>29</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D123" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="E123" s="16" t="s">
         <v>331</v>
-      </c>
-      <c r="E123" s="16" t="s">
-        <v>332</v>
       </c>
       <c r="F123" s="17"/>
       <c r="G123" s="18"/>
@@ -7358,13 +7388,13 @@
         <v>29</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D124" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="E124" s="16" t="s">
         <v>333</v>
-      </c>
-      <c r="E124" s="16" t="s">
-        <v>334</v>
       </c>
       <c r="F124" s="17"/>
       <c r="G124" s="18"/>
@@ -7387,13 +7417,13 @@
         <v>29</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D125" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="E125" s="16" t="s">
         <v>335</v>
-      </c>
-      <c r="E125" s="16" t="s">
-        <v>336</v>
       </c>
       <c r="F125" s="17"/>
       <c r="G125" s="18"/>
@@ -7416,13 +7446,13 @@
         <v>29</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D126" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="E126" s="16" t="s">
         <v>337</v>
-      </c>
-      <c r="E126" s="16" t="s">
-        <v>338</v>
       </c>
       <c r="F126" s="17"/>
       <c r="G126" s="18"/>
@@ -7445,13 +7475,13 @@
         <v>29</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D127" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="E127" s="16" t="s">
         <v>339</v>
-      </c>
-      <c r="E127" s="16" t="s">
-        <v>340</v>
       </c>
       <c r="F127" s="17"/>
       <c r="G127" s="18"/>
@@ -7474,13 +7504,13 @@
         <v>29</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D128" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="E128" s="16" t="s">
         <v>341</v>
-      </c>
-      <c r="E128" s="16" t="s">
-        <v>342</v>
       </c>
       <c r="F128" s="17"/>
       <c r="G128" s="18"/>
@@ -7503,13 +7533,13 @@
         <v>29</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D129" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="E129" s="16" t="s">
         <v>343</v>
-      </c>
-      <c r="E129" s="16" t="s">
-        <v>344</v>
       </c>
       <c r="F129" s="17"/>
       <c r="G129" s="18"/>
@@ -7532,13 +7562,13 @@
         <v>29</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D130" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="E130" s="16" t="s">
         <v>345</v>
-      </c>
-      <c r="E130" s="16" t="s">
-        <v>346</v>
       </c>
       <c r="F130" s="17"/>
       <c r="G130" s="18"/>
@@ -7561,13 +7591,13 @@
         <v>29</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D131" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="E131" s="16" t="s">
         <v>347</v>
-      </c>
-      <c r="E131" s="16" t="s">
-        <v>348</v>
       </c>
       <c r="F131" s="17"/>
       <c r="G131" s="18"/>
@@ -7590,13 +7620,13 @@
         <v>29</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D132" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="E132" s="16" t="s">
         <v>349</v>
-      </c>
-      <c r="E132" s="16" t="s">
-        <v>350</v>
       </c>
       <c r="F132" s="17"/>
       <c r="G132" s="18"/>
@@ -7619,13 +7649,13 @@
         <v>29</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D133" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="E133" s="16" t="s">
         <v>351</v>
-      </c>
-      <c r="E133" s="16" t="s">
-        <v>352</v>
       </c>
       <c r="F133" s="17"/>
       <c r="G133" s="18"/>
@@ -7648,13 +7678,13 @@
         <v>29</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D134" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="E134" s="16" t="s">
         <v>353</v>
-      </c>
-      <c r="E134" s="16" t="s">
-        <v>354</v>
       </c>
       <c r="F134" s="17"/>
       <c r="G134" s="18"/>
@@ -7677,13 +7707,13 @@
         <v>29</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D135" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="E135" s="16" t="s">
         <v>355</v>
-      </c>
-      <c r="E135" s="16" t="s">
-        <v>356</v>
       </c>
       <c r="F135" s="17"/>
       <c r="G135" s="18"/>
@@ -7706,13 +7736,13 @@
         <v>29</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D136" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="E136" s="16" t="s">
         <v>357</v>
-      </c>
-      <c r="E136" s="16" t="s">
-        <v>358</v>
       </c>
       <c r="F136" s="17"/>
       <c r="G136" s="18"/>
@@ -7735,13 +7765,13 @@
         <v>29</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D137" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="E137" s="16" t="s">
         <v>359</v>
-      </c>
-      <c r="E137" s="16" t="s">
-        <v>360</v>
       </c>
       <c r="F137" s="17"/>
       <c r="G137" s="18"/>
@@ -7764,13 +7794,13 @@
         <v>29</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D138" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="E138" s="16" t="s">
         <v>361</v>
-      </c>
-      <c r="E138" s="16" t="s">
-        <v>362</v>
       </c>
       <c r="F138" s="17"/>
       <c r="G138" s="18"/>
@@ -7793,13 +7823,13 @@
         <v>29</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D139" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="E139" s="16" t="s">
         <v>363</v>
-      </c>
-      <c r="E139" s="16" t="s">
-        <v>364</v>
       </c>
       <c r="F139" s="17"/>
       <c r="G139" s="18"/>
@@ -7822,13 +7852,13 @@
         <v>29</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D140" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="E140" s="16" t="s">
         <v>365</v>
-      </c>
-      <c r="E140" s="16" t="s">
-        <v>366</v>
       </c>
       <c r="F140" s="17"/>
       <c r="G140" s="18"/>
@@ -7851,13 +7881,13 @@
         <v>29</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D141" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="E141" s="16" t="s">
         <v>367</v>
-      </c>
-      <c r="E141" s="16" t="s">
-        <v>368</v>
       </c>
       <c r="F141" s="17"/>
       <c r="G141" s="18"/>
@@ -7880,13 +7910,13 @@
         <v>29</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D142" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="E142" s="16" t="s">
         <v>369</v>
-      </c>
-      <c r="E142" s="16" t="s">
-        <v>370</v>
       </c>
       <c r="F142" s="17"/>
       <c r="G142" s="18"/>
@@ -7909,13 +7939,13 @@
         <v>29</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D143" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="E143" s="16" t="s">
         <v>371</v>
-      </c>
-      <c r="E143" s="16" t="s">
-        <v>372</v>
       </c>
       <c r="F143" s="17"/>
       <c r="G143" s="18"/>
@@ -7938,13 +7968,13 @@
         <v>29</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D144" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="E144" s="16" t="s">
         <v>373</v>
-      </c>
-      <c r="E144" s="16" t="s">
-        <v>374</v>
       </c>
       <c r="F144" s="17"/>
       <c r="G144" s="18"/>
@@ -7967,13 +7997,13 @@
         <v>29</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D145" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="E145" s="16" t="s">
         <v>375</v>
-      </c>
-      <c r="E145" s="16" t="s">
-        <v>376</v>
       </c>
       <c r="F145" s="17"/>
       <c r="G145" s="18"/>
@@ -7996,13 +8026,13 @@
         <v>29</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D146" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="E146" s="16" t="s">
         <v>377</v>
-      </c>
-      <c r="E146" s="16" t="s">
-        <v>378</v>
       </c>
       <c r="F146" s="17"/>
       <c r="G146" s="18"/>
@@ -8025,13 +8055,13 @@
         <v>29</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D147" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="E147" s="16" t="s">
         <v>379</v>
-      </c>
-      <c r="E147" s="16" t="s">
-        <v>380</v>
       </c>
       <c r="F147" s="17"/>
       <c r="G147" s="18"/>
@@ -18233,7 +18263,7 @@
   <dimension ref="A1:D998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -18254,10 +18284,10 @@
         <v>15</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>381</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
@@ -18265,13 +18295,13 @@
         <v>30</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="D2" s="28" t="s">
         <v>384</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
@@ -18279,13 +18309,13 @@
         <v>41</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C3" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>386</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
@@ -18293,55 +18323,55 @@
         <v>58</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C4" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>388</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C5" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>390</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C6" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>392</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1">
       <c r="A7" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C7" s="35" t="s">
+        <v>393</v>
+      </c>
+      <c r="D7" s="32" t="s">
         <v>394</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1"/>
@@ -19372,7 +19402,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>52</v>
@@ -20389,15 +20419,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA9DE3DB3C6091468D1D4005047F3381" ma:contentTypeVersion="4" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="459c8a6a3a88bd262a2ff1f0ba7a9f11">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ae8219d-8505-4e64-b47a-e5e02bd99ff8" xmlns:ns3="b6c6c545-4433-4453-a388-ae81a1a09069" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd389b9c591f38f50631ea74e6d4f129" ns2:_="" ns3:_="">
     <xsd:import namespace="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
@@ -20562,10 +20583,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44D316A-03D1-4D0D-8C30-961F2644D409}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D083E07-CB22-4B29-AE20-400E2F1FBB78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
+    <ds:schemaRef ds:uri="b6c6c545-4433-4453-a388-ae81a1a09069"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D083E07-CB22-4B29-AE20-400E2F1FBB78}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44D316A-03D1-4D0D-8C30-961F2644D409}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Corretto i files excel come richiesto per i test marcati FAIL
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.0/report-checklist.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\accreditamento\Accreditamento CLINICO\S1#060000000000XX\INSIEL\CLINICO\G4.3.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\fse_new\accreditamento\CLINICO\FORK\it-fse-accreditamento\GATEWAY\S1#060000000000XX\INSIEL\CLINICO\G4.3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7276E4B-CCD1-4269-8900-6E69C59C7A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E96A32C-2F55-4CC4-9288-A6BFDA3B5C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3586,10 +3586,10 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L64" sqref="L64"/>
+      <selection pane="bottomRight" activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -5445,7 +5445,7 @@
         <v>48</v>
       </c>
       <c r="L65" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M65" s="19"/>
       <c r="N65" s="20" t="s">
@@ -5488,7 +5488,7 @@
         <v>48</v>
       </c>
       <c r="L66" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="N66" s="20" t="s">
         <v>48</v>
@@ -5563,7 +5563,7 @@
         <v>48</v>
       </c>
       <c r="L68" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M68" s="19"/>
       <c r="N68" s="20" t="s">
@@ -5606,7 +5606,7 @@
         <v>48</v>
       </c>
       <c r="L69" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M69" s="19"/>
       <c r="N69" s="20" t="s">
@@ -5648,8 +5648,8 @@
       <c r="K70" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="L70" s="37" t="s">
-        <v>151</v>
+      <c r="L70" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="M70" s="19"/>
       <c r="N70" s="20" t="s">
@@ -5692,7 +5692,7 @@
         <v>48</v>
       </c>
       <c r="L71" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M71" s="19"/>
       <c r="N71" s="20" t="s">
@@ -5900,7 +5900,7 @@
         <v>48</v>
       </c>
       <c r="L77" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M77" s="19"/>
       <c r="N77" s="20" t="s">
@@ -5943,7 +5943,7 @@
         <v>48</v>
       </c>
       <c r="L78" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M78" s="19"/>
       <c r="N78" s="20" t="s">
@@ -6019,7 +6019,7 @@
         <v>48</v>
       </c>
       <c r="L80" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M80" s="19"/>
       <c r="N80" s="20" t="s">
@@ -6062,7 +6062,7 @@
         <v>48</v>
       </c>
       <c r="L81" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M81" s="19"/>
       <c r="N81" s="20" t="s">
@@ -6138,7 +6138,7 @@
         <v>48</v>
       </c>
       <c r="L83" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M83" s="19"/>
       <c r="N83" s="20" t="s">
@@ -6181,7 +6181,7 @@
         <v>48</v>
       </c>
       <c r="L84" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M84" s="19"/>
       <c r="N84" s="20" t="s">
@@ -6224,7 +6224,7 @@
         <v>48</v>
       </c>
       <c r="L85" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M85" s="19"/>
       <c r="N85" s="20" t="s">
@@ -6267,7 +6267,7 @@
         <v>48</v>
       </c>
       <c r="L86" s="19" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="M86" s="19"/>
       <c r="N86" s="20" t="s">
@@ -20419,6 +20419,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA9DE3DB3C6091468D1D4005047F3381" ma:contentTypeVersion="4" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="459c8a6a3a88bd262a2ff1f0ba7a9f11">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ae8219d-8505-4e64-b47a-e5e02bd99ff8" xmlns:ns3="b6c6c545-4433-4453-a388-ae81a1a09069" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd389b9c591f38f50631ea74e6d4f129" ns2:_="" ns3:_="">
     <xsd:import namespace="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
@@ -20583,16 +20592,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44D316A-03D1-4D0D-8C30-961F2644D409}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D083E07-CB22-4B29-AE20-400E2F1FBB78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20609,12 +20617,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44D316A-03D1-4D0D-8C30-961F2644D409}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiornato i file excel e json come richiesto
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.0/report-checklist.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\fse_new\accreditamento\CLINICO\FORK\it-fse-accreditamento\GATEWAY\S1#060000000000XX\INSIEL\CLINICO\G4.3.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\fse_new\accreditamento\FORK\it-fse-accreditamento\GATEWAY\S1#060000000000XX\INSIEL\CLINICO\G4.3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E96A32C-2F55-4CC4-9288-A6BFDA3B5C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E2838E-72F6-4FB2-9354-34AC53D247FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="397">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2515,11 +2515,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="194.140625" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="194.109375" customWidth="1"/>
+    <col min="3" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -3586,27 +3586,27 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L71" sqref="L71"/>
+      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
-    <col min="5" max="5" width="104.7109375" customWidth="1"/>
-    <col min="6" max="9" width="33.28515625" customWidth="1"/>
-    <col min="10" max="10" width="35.7109375" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" customWidth="1"/>
-    <col min="12" max="12" width="33.28515625" customWidth="1"/>
-    <col min="13" max="13" width="36.42578125" style="41" customWidth="1"/>
-    <col min="14" max="14" width="36.42578125" customWidth="1"/>
-    <col min="15" max="15" width="31.7109375" customWidth="1"/>
-    <col min="16" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="63.88671875" customWidth="1"/>
+    <col min="5" max="5" width="104.6640625" customWidth="1"/>
+    <col min="6" max="9" width="33.33203125" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" customWidth="1"/>
+    <col min="12" max="12" width="33.33203125" customWidth="1"/>
+    <col min="13" max="13" width="36.44140625" style="41" customWidth="1"/>
+    <col min="14" max="14" width="36.44140625" customWidth="1"/>
+    <col min="15" max="15" width="31.6640625" customWidth="1"/>
+    <col min="16" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3621,7 +3621,7 @@
       <c r="N1" s="9"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="18.75">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" s="46" t="s">
         <v>8</v>
       </c>
@@ -3641,7 +3641,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="6"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="15.6">
       <c r="A3" s="49" t="s">
         <v>10</v>
       </c>
@@ -3661,7 +3661,7 @@
       <c r="N3" s="9"/>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.6">
       <c r="A4" s="51"/>
       <c r="B4" s="52"/>
       <c r="C4" s="55" t="s">
@@ -3680,7 +3680,7 @@
       <c r="N4" s="9"/>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.6">
       <c r="A5" s="53"/>
       <c r="B5" s="54"/>
       <c r="C5" s="55" t="s">
@@ -3728,7 +3728,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+    <row r="8" spans="1:15" ht="15" thickBot="1">
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -3740,7 +3740,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="19.5" thickBot="1">
+    <row r="9" spans="1:15" ht="18.600000000000001" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="165.75" hidden="1" thickBot="1">
+    <row r="10" spans="1:15" ht="144.6" hidden="1" thickBot="1">
       <c r="A10" s="14">
         <v>1</v>
       </c>
@@ -3814,7 +3814,7 @@
       <c r="N10" s="20"/>
       <c r="O10" s="21"/>
     </row>
-    <row r="11" spans="1:15" ht="165.75" hidden="1" thickBot="1">
+    <row r="11" spans="1:15" ht="144.6" hidden="1" thickBot="1">
       <c r="A11" s="14">
         <v>2</v>
       </c>
@@ -3841,7 +3841,7 @@
       <c r="N11" s="20"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="1:15" ht="165.75" hidden="1" thickBot="1">
+    <row r="12" spans="1:15" ht="144.6" hidden="1" thickBot="1">
       <c r="A12" s="14">
         <v>3</v>
       </c>
@@ -3868,7 +3868,7 @@
       <c r="N12" s="20"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="1:15" ht="165.75" hidden="1" thickBot="1">
+    <row r="13" spans="1:15" ht="144.6" hidden="1" thickBot="1">
       <c r="A13" s="14">
         <v>4</v>
       </c>
@@ -3895,7 +3895,7 @@
       <c r="N13" s="20"/>
       <c r="O13" s="21"/>
     </row>
-    <row r="14" spans="1:15" ht="165.75" hidden="1" thickBot="1">
+    <row r="14" spans="1:15" ht="144.6" hidden="1" thickBot="1">
       <c r="A14" s="14">
         <v>5</v>
       </c>
@@ -3922,7 +3922,7 @@
       <c r="N14" s="20"/>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="1:15" ht="150.75" thickBot="1">
+    <row r="15" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A15" s="14">
         <v>6</v>
       </c>
@@ -3961,7 +3961,7 @@
       <c r="N15" s="20"/>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="1:15" ht="150.75" thickBot="1">
+    <row r="16" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A16" s="14">
         <v>7</v>
       </c>
@@ -3992,7 +3992,7 @@
       <c r="N16" s="20"/>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="1:15" ht="150.75" thickBot="1">
+    <row r="17" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A17" s="14">
         <v>8</v>
       </c>
@@ -4023,7 +4023,7 @@
       <c r="N17" s="20"/>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="1:15" ht="150.75" thickBot="1">
+    <row r="18" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A18" s="14">
         <v>9</v>
       </c>
@@ -4054,7 +4054,7 @@
       <c r="N18" s="20"/>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="1:15" ht="135.75" thickBot="1">
+    <row r="19" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A19" s="14">
         <v>11</v>
       </c>
@@ -4093,7 +4093,7 @@
       <c r="N19" s="20"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="1:15" ht="135.75" thickBot="1">
+    <row r="20" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A20" s="14">
         <v>12</v>
       </c>
@@ -4124,7 +4124,7 @@
       <c r="N20" s="20"/>
       <c r="O20" s="21"/>
     </row>
-    <row r="21" spans="1:15" ht="135.75" thickBot="1">
+    <row r="21" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A21" s="14">
         <v>13</v>
       </c>
@@ -4155,7 +4155,7 @@
       <c r="N21" s="20"/>
       <c r="O21" s="21"/>
     </row>
-    <row r="22" spans="1:15" ht="135.75" thickBot="1">
+    <row r="22" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A22" s="14">
         <v>14</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="N22" s="20"/>
       <c r="O22" s="21"/>
     </row>
-    <row r="23" spans="1:15" ht="135.75" hidden="1" thickBot="1">
+    <row r="23" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A23" s="14">
         <v>16</v>
       </c>
@@ -4213,7 +4213,7 @@
       <c r="N23" s="20"/>
       <c r="O23" s="21"/>
     </row>
-    <row r="24" spans="1:15" ht="135.75" hidden="1" thickBot="1">
+    <row r="24" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A24" s="14">
         <v>17</v>
       </c>
@@ -4240,7 +4240,7 @@
       <c r="N24" s="20"/>
       <c r="O24" s="21"/>
     </row>
-    <row r="25" spans="1:15" ht="135.75" hidden="1" thickBot="1">
+    <row r="25" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A25" s="14">
         <v>18</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="N25" s="20"/>
       <c r="O25" s="21"/>
     </row>
-    <row r="26" spans="1:15" ht="135.75" hidden="1" thickBot="1">
+    <row r="26" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A26" s="14">
         <v>19</v>
       </c>
@@ -4294,7 +4294,7 @@
       <c r="N26" s="20"/>
       <c r="O26" s="21"/>
     </row>
-    <row r="27" spans="1:15" ht="150.75" hidden="1" thickBot="1">
+    <row r="27" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A27" s="14">
         <v>20</v>
       </c>
@@ -4321,7 +4321,7 @@
       <c r="N27" s="20"/>
       <c r="O27" s="21"/>
     </row>
-    <row r="28" spans="1:15" ht="150.75" hidden="1" thickBot="1">
+    <row r="28" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A28" s="14">
         <v>21</v>
       </c>
@@ -4348,7 +4348,7 @@
       <c r="N28" s="20"/>
       <c r="O28" s="21"/>
     </row>
-    <row r="29" spans="1:15" ht="150.75" hidden="1" thickBot="1">
+    <row r="29" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A29" s="14">
         <v>22</v>
       </c>
@@ -4375,7 +4375,7 @@
       <c r="N29" s="20"/>
       <c r="O29" s="21"/>
     </row>
-    <row r="30" spans="1:15" ht="150.75" hidden="1" thickBot="1">
+    <row r="30" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A30" s="14">
         <v>23</v>
       </c>
@@ -4402,7 +4402,7 @@
       <c r="N30" s="20"/>
       <c r="O30" s="21"/>
     </row>
-    <row r="31" spans="1:15" ht="150.75" hidden="1" thickBot="1">
+    <row r="31" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A31" s="14">
         <v>24</v>
       </c>
@@ -4429,7 +4429,7 @@
       <c r="N31" s="20"/>
       <c r="O31" s="21"/>
     </row>
-    <row r="32" spans="1:15" ht="150.75" hidden="1" thickBot="1">
+    <row r="32" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A32" s="14">
         <v>25</v>
       </c>
@@ -4456,7 +4456,7 @@
       <c r="N32" s="20"/>
       <c r="O32" s="21"/>
     </row>
-    <row r="33" spans="1:15" ht="150.75" hidden="1" thickBot="1">
+    <row r="33" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A33" s="14">
         <v>26</v>
       </c>
@@ -4483,7 +4483,7 @@
       <c r="N33" s="20"/>
       <c r="O33" s="21"/>
     </row>
-    <row r="34" spans="1:15" ht="150.75" hidden="1" thickBot="1">
+    <row r="34" spans="1:15" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A34" s="14">
         <v>27</v>
       </c>
@@ -4510,7 +4510,7 @@
       <c r="N34" s="20"/>
       <c r="O34" s="21"/>
     </row>
-    <row r="35" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="35" spans="1:15" ht="101.4" hidden="1" thickBot="1">
       <c r="A35" s="14">
         <v>28</v>
       </c>
@@ -4539,7 +4539,7 @@
       </c>
       <c r="O35" s="21"/>
     </row>
-    <row r="36" spans="1:15" ht="120.75" thickBot="1">
+    <row r="36" spans="1:15" ht="101.4" thickBot="1">
       <c r="A36" s="14">
         <v>29</v>
       </c>
@@ -4572,7 +4572,7 @@
       </c>
       <c r="O36" s="21"/>
     </row>
-    <row r="37" spans="1:15" ht="120.75" thickBot="1">
+    <row r="37" spans="1:15" ht="101.4" thickBot="1">
       <c r="A37" s="14">
         <v>31</v>
       </c>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="O37" s="21"/>
     </row>
-    <row r="38" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="38" spans="1:15" ht="101.4" hidden="1" thickBot="1">
       <c r="A38" s="14">
         <v>33</v>
       </c>
@@ -4634,7 +4634,7 @@
       </c>
       <c r="O38" s="21"/>
     </row>
-    <row r="39" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="39" spans="1:15" ht="101.4" hidden="1" thickBot="1">
       <c r="A39" s="14">
         <v>34</v>
       </c>
@@ -4663,7 +4663,7 @@
       </c>
       <c r="O39" s="21"/>
     </row>
-    <row r="40" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="40" spans="1:15" ht="101.4" hidden="1" thickBot="1">
       <c r="A40" s="14">
         <v>35</v>
       </c>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="O40" s="21"/>
     </row>
-    <row r="41" spans="1:15" ht="135.75" hidden="1" thickBot="1">
+    <row r="41" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A41" s="14">
         <v>36</v>
       </c>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="O41" s="21"/>
     </row>
-    <row r="42" spans="1:15" ht="135.75" thickBot="1">
+    <row r="42" spans="1:15" ht="115.8" thickBot="1">
       <c r="A42" s="14">
         <v>37</v>
       </c>
@@ -4754,7 +4754,7 @@
       </c>
       <c r="O42" s="21"/>
     </row>
-    <row r="43" spans="1:15" ht="135.75" thickBot="1">
+    <row r="43" spans="1:15" ht="115.8" thickBot="1">
       <c r="A43" s="14">
         <v>39</v>
       </c>
@@ -4787,7 +4787,7 @@
       </c>
       <c r="O43" s="21"/>
     </row>
-    <row r="44" spans="1:15" ht="135.75" hidden="1" thickBot="1">
+    <row r="44" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A44" s="14">
         <v>41</v>
       </c>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="O44" s="21"/>
     </row>
-    <row r="45" spans="1:15" ht="135.75" hidden="1" thickBot="1">
+    <row r="45" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A45" s="14">
         <v>42</v>
       </c>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="O45" s="21"/>
     </row>
-    <row r="46" spans="1:15" ht="135.75" hidden="1" thickBot="1">
+    <row r="46" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A46" s="14">
         <v>43</v>
       </c>
@@ -4874,7 +4874,7 @@
       </c>
       <c r="O46" s="21"/>
     </row>
-    <row r="47" spans="1:15" ht="45.75" hidden="1" thickBot="1">
+    <row r="47" spans="1:15" ht="43.8" hidden="1" thickBot="1">
       <c r="A47" s="14">
         <v>44</v>
       </c>
@@ -4903,7 +4903,7 @@
       </c>
       <c r="O47" s="21"/>
     </row>
-    <row r="48" spans="1:15" ht="45.75" thickBot="1">
+    <row r="48" spans="1:15" ht="43.8" thickBot="1">
       <c r="A48" s="14">
         <v>45</v>
       </c>
@@ -4938,7 +4938,7 @@
       </c>
       <c r="O48" s="21"/>
     </row>
-    <row r="49" spans="1:15" ht="45.75" thickBot="1">
+    <row r="49" spans="1:15" ht="43.8" thickBot="1">
       <c r="A49" s="14">
         <v>47</v>
       </c>
@@ -4973,7 +4973,7 @@
       </c>
       <c r="O49" s="21"/>
     </row>
-    <row r="50" spans="1:15" ht="45.75" hidden="1" thickBot="1">
+    <row r="50" spans="1:15" ht="43.8" hidden="1" thickBot="1">
       <c r="A50" s="14">
         <v>49</v>
       </c>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="O50" s="21"/>
     </row>
-    <row r="51" spans="1:15" ht="45.75" hidden="1" thickBot="1">
+    <row r="51" spans="1:15" ht="43.8" hidden="1" thickBot="1">
       <c r="A51" s="14">
         <v>50</v>
       </c>
@@ -5031,7 +5031,7 @@
       </c>
       <c r="O51" s="21"/>
     </row>
-    <row r="52" spans="1:15" ht="45.75" hidden="1" thickBot="1">
+    <row r="52" spans="1:15" ht="43.8" hidden="1" thickBot="1">
       <c r="A52" s="14">
         <v>51</v>
       </c>
@@ -5060,7 +5060,7 @@
       </c>
       <c r="O52" s="21"/>
     </row>
-    <row r="53" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="53" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A53" s="14">
         <v>52</v>
       </c>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="O53" s="21"/>
     </row>
-    <row r="54" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="54" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A54" s="14">
         <v>53</v>
       </c>
@@ -5118,7 +5118,7 @@
       </c>
       <c r="O54" s="21"/>
     </row>
-    <row r="55" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="55" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A55" s="14">
         <v>54</v>
       </c>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="O55" s="21"/>
     </row>
-    <row r="56" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="56" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A56" s="14">
         <v>55</v>
       </c>
@@ -5176,7 +5176,7 @@
       </c>
       <c r="O56" s="21"/>
     </row>
-    <row r="57" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="57" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A57" s="14">
         <v>56</v>
       </c>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="O57" s="21"/>
     </row>
-    <row r="58" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="58" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A58" s="14">
         <v>57</v>
       </c>
@@ -5234,7 +5234,7 @@
       </c>
       <c r="O58" s="21"/>
     </row>
-    <row r="59" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="59" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A59" s="14">
         <v>58</v>
       </c>
@@ -5263,7 +5263,7 @@
       </c>
       <c r="O59" s="21"/>
     </row>
-    <row r="60" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="60" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A60" s="14">
         <v>59</v>
       </c>
@@ -5292,7 +5292,7 @@
       </c>
       <c r="O60" s="21"/>
     </row>
-    <row r="61" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="61" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A61" s="14">
         <v>60</v>
       </c>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="O61" s="21"/>
     </row>
-    <row r="62" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="62" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A62" s="14">
         <v>61</v>
       </c>
@@ -5350,7 +5350,7 @@
       </c>
       <c r="O62" s="21"/>
     </row>
-    <row r="63" spans="1:15" ht="120.75" hidden="1" thickBot="1">
+    <row r="63" spans="1:15" ht="115.8" hidden="1" thickBot="1">
       <c r="A63" s="14">
         <v>62</v>
       </c>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="O63" s="21"/>
     </row>
-    <row r="64" spans="1:15" ht="120.75" thickBot="1">
+    <row r="64" spans="1:15" ht="115.8" thickBot="1">
       <c r="A64" s="14">
         <v>63</v>
       </c>
@@ -5407,10 +5407,12 @@
       <c r="M64" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="N64" s="20"/>
+      <c r="N64" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="O64" s="21"/>
     </row>
-    <row r="65" spans="1:15" ht="120.75" thickBot="1">
+    <row r="65" spans="1:15" ht="115.8" thickBot="1">
       <c r="A65" s="14">
         <v>64</v>
       </c>
@@ -5453,7 +5455,7 @@
       </c>
       <c r="O65" s="21"/>
     </row>
-    <row r="66" spans="1:15" ht="120.75" thickBot="1">
+    <row r="66" spans="1:15" ht="115.8" thickBot="1">
       <c r="A66" s="14">
         <v>65</v>
       </c>
@@ -5495,7 +5497,7 @@
       </c>
       <c r="O66" s="21"/>
     </row>
-    <row r="67" spans="1:15" ht="120.75" thickBot="1">
+    <row r="67" spans="1:15" ht="115.8" thickBot="1">
       <c r="A67" s="14">
         <v>66</v>
       </c>
@@ -5528,7 +5530,7 @@
       </c>
       <c r="O67" s="21"/>
     </row>
-    <row r="68" spans="1:15" ht="120.75" thickBot="1">
+    <row r="68" spans="1:15" ht="115.8" thickBot="1">
       <c r="A68" s="14">
         <v>67</v>
       </c>
@@ -5571,7 +5573,7 @@
       </c>
       <c r="O68" s="21"/>
     </row>
-    <row r="69" spans="1:15" ht="120.75" thickBot="1">
+    <row r="69" spans="1:15" ht="115.8" thickBot="1">
       <c r="A69" s="14">
         <v>68</v>
       </c>
@@ -5657,7 +5659,7 @@
       </c>
       <c r="O70" s="21"/>
     </row>
-    <row r="71" spans="1:15" ht="120.75" thickBot="1">
+    <row r="71" spans="1:15" ht="115.8" thickBot="1">
       <c r="A71" s="14">
         <v>70</v>
       </c>
@@ -5700,7 +5702,7 @@
       </c>
       <c r="O71" s="21"/>
     </row>
-    <row r="72" spans="1:15" ht="120.75" thickBot="1">
+    <row r="72" spans="1:15" ht="115.8" thickBot="1">
       <c r="A72" s="14">
         <v>71</v>
       </c>
@@ -5733,7 +5735,7 @@
       </c>
       <c r="O72" s="21"/>
     </row>
-    <row r="73" spans="1:15" ht="120.75" thickBot="1">
+    <row r="73" spans="1:15" ht="115.8" thickBot="1">
       <c r="A73" s="14">
         <v>72</v>
       </c>
@@ -5766,7 +5768,7 @@
       </c>
       <c r="O73" s="21"/>
     </row>
-    <row r="74" spans="1:15" ht="120.75" thickBot="1">
+    <row r="74" spans="1:15" ht="115.8" thickBot="1">
       <c r="A74" s="14">
         <v>73</v>
       </c>
@@ -5799,7 +5801,7 @@
       </c>
       <c r="O74" s="21"/>
     </row>
-    <row r="75" spans="1:15" ht="120.75" thickBot="1">
+    <row r="75" spans="1:15" ht="115.8" thickBot="1">
       <c r="A75" s="14">
         <v>74</v>
       </c>
@@ -5832,7 +5834,7 @@
       </c>
       <c r="O75" s="21"/>
     </row>
-    <row r="76" spans="1:15" ht="135.75" thickBot="1">
+    <row r="76" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A76" s="14">
         <v>75</v>
       </c>
@@ -5865,7 +5867,7 @@
       </c>
       <c r="O76" s="21"/>
     </row>
-    <row r="77" spans="1:15" ht="180.75" thickBot="1">
+    <row r="77" spans="1:15" ht="159" thickBot="1">
       <c r="A77" s="14">
         <v>76</v>
       </c>
@@ -5908,7 +5910,7 @@
       </c>
       <c r="O77" s="21"/>
     </row>
-    <row r="78" spans="1:15" ht="225.75" thickBot="1">
+    <row r="78" spans="1:15" ht="187.8" thickBot="1">
       <c r="A78" s="14">
         <v>77</v>
       </c>
@@ -5951,7 +5953,7 @@
       </c>
       <c r="O78" s="21"/>
     </row>
-    <row r="79" spans="1:15" ht="105.75" thickBot="1">
+    <row r="79" spans="1:15" ht="101.4" thickBot="1">
       <c r="A79" s="14">
         <v>78</v>
       </c>
@@ -5984,7 +5986,7 @@
       </c>
       <c r="O79" s="21"/>
     </row>
-    <row r="80" spans="1:15" ht="225.75" thickBot="1">
+    <row r="80" spans="1:15" ht="187.8" thickBot="1">
       <c r="A80" s="14">
         <v>79</v>
       </c>
@@ -6027,7 +6029,7 @@
       </c>
       <c r="O80" s="21"/>
     </row>
-    <row r="81" spans="1:15" ht="120.75" thickBot="1">
+    <row r="81" spans="1:15" ht="115.8" thickBot="1">
       <c r="A81" s="14">
         <v>80</v>
       </c>
@@ -6070,7 +6072,7 @@
       </c>
       <c r="O81" s="21"/>
     </row>
-    <row r="82" spans="1:15" ht="120.75" thickBot="1">
+    <row r="82" spans="1:15" ht="115.8" thickBot="1">
       <c r="A82" s="14">
         <v>81</v>
       </c>
@@ -6103,7 +6105,7 @@
       </c>
       <c r="O82" s="21"/>
     </row>
-    <row r="83" spans="1:15" ht="315.75" thickBot="1">
+    <row r="83" spans="1:15" ht="274.2" thickBot="1">
       <c r="A83" s="14">
         <v>82</v>
       </c>
@@ -6146,7 +6148,7 @@
       </c>
       <c r="O83" s="21"/>
     </row>
-    <row r="84" spans="1:15" ht="225.75" thickBot="1">
+    <row r="84" spans="1:15" ht="202.2" thickBot="1">
       <c r="A84" s="14">
         <v>83</v>
       </c>
@@ -6189,7 +6191,7 @@
       </c>
       <c r="O84" s="21"/>
     </row>
-    <row r="85" spans="1:15" ht="135.75" thickBot="1">
+    <row r="85" spans="1:15" ht="115.8" thickBot="1">
       <c r="A85" s="14">
         <v>84</v>
       </c>
@@ -6232,7 +6234,7 @@
       </c>
       <c r="O85" s="21"/>
     </row>
-    <row r="86" spans="1:15" ht="210.75" thickBot="1">
+    <row r="86" spans="1:15" ht="187.8" thickBot="1">
       <c r="A86" s="14">
         <v>85</v>
       </c>
@@ -6275,7 +6277,7 @@
       </c>
       <c r="O86" s="21"/>
     </row>
-    <row r="87" spans="1:15" ht="120.75" thickBot="1">
+    <row r="87" spans="1:15" ht="115.8" thickBot="1">
       <c r="A87" s="14">
         <v>86</v>
       </c>
@@ -6308,7 +6310,7 @@
       </c>
       <c r="O87" s="21"/>
     </row>
-    <row r="88" spans="1:15" ht="135.75" thickBot="1">
+    <row r="88" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A88" s="14">
         <v>87</v>
       </c>
@@ -6341,7 +6343,7 @@
       </c>
       <c r="O88" s="21"/>
     </row>
-    <row r="89" spans="1:15" ht="120.75" thickBot="1">
+    <row r="89" spans="1:15" ht="115.8" thickBot="1">
       <c r="A89" s="14">
         <v>88</v>
       </c>
@@ -6374,7 +6376,7 @@
       </c>
       <c r="O89" s="21"/>
     </row>
-    <row r="90" spans="1:15" ht="105.75" thickBot="1">
+    <row r="90" spans="1:15" ht="101.4" thickBot="1">
       <c r="A90" s="14">
         <v>89</v>
       </c>
@@ -6407,7 +6409,7 @@
       </c>
       <c r="O90" s="21"/>
     </row>
-    <row r="91" spans="1:15" ht="105.75" thickBot="1">
+    <row r="91" spans="1:15" ht="101.4" thickBot="1">
       <c r="A91" s="14">
         <v>90</v>
       </c>
@@ -6440,7 +6442,7 @@
       </c>
       <c r="O91" s="21"/>
     </row>
-    <row r="92" spans="1:15" ht="120.75" thickBot="1">
+    <row r="92" spans="1:15" ht="115.8" thickBot="1">
       <c r="A92" s="14">
         <v>91</v>
       </c>
@@ -6473,7 +6475,7 @@
       </c>
       <c r="O92" s="21"/>
     </row>
-    <row r="93" spans="1:15" ht="120.75" thickBot="1">
+    <row r="93" spans="1:15" ht="115.8" thickBot="1">
       <c r="A93" s="14">
         <v>92</v>
       </c>
@@ -6506,7 +6508,7 @@
       </c>
       <c r="O93" s="21"/>
     </row>
-    <row r="94" spans="1:15" ht="120">
+    <row r="94" spans="1:15" ht="115.2">
       <c r="A94" s="14">
         <v>93</v>
       </c>
@@ -6539,7 +6541,7 @@
       </c>
       <c r="O94" s="21"/>
     </row>
-    <row r="95" spans="1:15" ht="135" hidden="1">
+    <row r="95" spans="1:15" ht="129.6" hidden="1">
       <c r="A95" s="14">
         <v>94</v>
       </c>
@@ -6568,7 +6570,7 @@
       </c>
       <c r="O95" s="21"/>
     </row>
-    <row r="96" spans="1:15" ht="135" hidden="1">
+    <row r="96" spans="1:15" ht="129.6" hidden="1">
       <c r="A96" s="14">
         <v>95</v>
       </c>
@@ -6597,7 +6599,7 @@
       </c>
       <c r="O96" s="21"/>
     </row>
-    <row r="97" spans="1:15" ht="105" hidden="1">
+    <row r="97" spans="1:15" ht="100.8" hidden="1">
       <c r="A97" s="14">
         <v>96</v>
       </c>
@@ -6626,7 +6628,7 @@
       </c>
       <c r="O97" s="21"/>
     </row>
-    <row r="98" spans="1:15" ht="120" hidden="1">
+    <row r="98" spans="1:15" ht="115.2" hidden="1">
       <c r="A98" s="14">
         <v>97</v>
       </c>
@@ -6655,7 +6657,7 @@
       </c>
       <c r="O98" s="21"/>
     </row>
-    <row r="99" spans="1:15" ht="135" hidden="1">
+    <row r="99" spans="1:15" ht="129.6" hidden="1">
       <c r="A99" s="14">
         <v>98</v>
       </c>
@@ -6684,7 +6686,7 @@
       </c>
       <c r="O99" s="21"/>
     </row>
-    <row r="100" spans="1:15" ht="135" hidden="1">
+    <row r="100" spans="1:15" ht="129.6" hidden="1">
       <c r="A100" s="14">
         <v>99</v>
       </c>
@@ -6713,7 +6715,7 @@
       </c>
       <c r="O100" s="21"/>
     </row>
-    <row r="101" spans="1:15" ht="105" hidden="1">
+    <row r="101" spans="1:15" ht="100.8" hidden="1">
       <c r="A101" s="14">
         <v>100</v>
       </c>
@@ -6742,7 +6744,7 @@
       </c>
       <c r="O101" s="21"/>
     </row>
-    <row r="102" spans="1:15" ht="120" hidden="1">
+    <row r="102" spans="1:15" ht="115.2" hidden="1">
       <c r="A102" s="14">
         <v>101</v>
       </c>
@@ -6771,7 +6773,7 @@
       </c>
       <c r="O102" s="21"/>
     </row>
-    <row r="103" spans="1:15" ht="135" hidden="1">
+    <row r="103" spans="1:15" ht="129.6" hidden="1">
       <c r="A103" s="14">
         <v>102</v>
       </c>
@@ -6800,7 +6802,7 @@
       </c>
       <c r="O103" s="21"/>
     </row>
-    <row r="104" spans="1:15" ht="135" hidden="1">
+    <row r="104" spans="1:15" ht="129.6" hidden="1">
       <c r="A104" s="14">
         <v>103</v>
       </c>
@@ -6829,7 +6831,7 @@
       </c>
       <c r="O104" s="21"/>
     </row>
-    <row r="105" spans="1:15" ht="105" hidden="1">
+    <row r="105" spans="1:15" ht="100.8" hidden="1">
       <c r="A105" s="14">
         <v>104</v>
       </c>
@@ -6858,7 +6860,7 @@
       </c>
       <c r="O105" s="21"/>
     </row>
-    <row r="106" spans="1:15" ht="135" hidden="1">
+    <row r="106" spans="1:15" ht="129.6" hidden="1">
       <c r="A106" s="14">
         <v>105</v>
       </c>
@@ -6887,7 +6889,7 @@
       </c>
       <c r="O106" s="21"/>
     </row>
-    <row r="107" spans="1:15" ht="135" hidden="1">
+    <row r="107" spans="1:15" ht="129.6" hidden="1">
       <c r="A107" s="14">
         <v>106</v>
       </c>
@@ -6916,7 +6918,7 @@
       </c>
       <c r="O107" s="21"/>
     </row>
-    <row r="108" spans="1:15" ht="120" hidden="1">
+    <row r="108" spans="1:15" ht="115.2" hidden="1">
       <c r="A108" s="14">
         <v>107</v>
       </c>
@@ -6945,7 +6947,7 @@
       </c>
       <c r="O108" s="21"/>
     </row>
-    <row r="109" spans="1:15" ht="120" hidden="1">
+    <row r="109" spans="1:15" ht="115.2" hidden="1">
       <c r="A109" s="14">
         <v>108</v>
       </c>
@@ -6974,7 +6976,7 @@
       </c>
       <c r="O109" s="21"/>
     </row>
-    <row r="110" spans="1:15" ht="120" hidden="1">
+    <row r="110" spans="1:15" ht="115.2" hidden="1">
       <c r="A110" s="14">
         <v>109</v>
       </c>
@@ -7003,7 +7005,7 @@
       </c>
       <c r="O110" s="21"/>
     </row>
-    <row r="111" spans="1:15" ht="105" hidden="1">
+    <row r="111" spans="1:15" ht="100.8" hidden="1">
       <c r="A111" s="14">
         <v>110</v>
       </c>
@@ -7032,7 +7034,7 @@
       </c>
       <c r="O111" s="21"/>
     </row>
-    <row r="112" spans="1:15" ht="120" hidden="1">
+    <row r="112" spans="1:15" ht="115.2" hidden="1">
       <c r="A112" s="14">
         <v>111</v>
       </c>
@@ -7061,7 +7063,7 @@
       </c>
       <c r="O112" s="21"/>
     </row>
-    <row r="113" spans="1:15" ht="120" hidden="1">
+    <row r="113" spans="1:15" ht="115.2" hidden="1">
       <c r="A113" s="14">
         <v>112</v>
       </c>
@@ -7090,7 +7092,7 @@
       </c>
       <c r="O113" s="21"/>
     </row>
-    <row r="114" spans="1:15" ht="120" hidden="1">
+    <row r="114" spans="1:15" ht="115.2" hidden="1">
       <c r="A114" s="14">
         <v>113</v>
       </c>
@@ -7119,7 +7121,7 @@
       </c>
       <c r="O114" s="21"/>
     </row>
-    <row r="115" spans="1:15" ht="120" hidden="1">
+    <row r="115" spans="1:15" ht="115.2" hidden="1">
       <c r="A115" s="14">
         <v>114</v>
       </c>
@@ -7148,7 +7150,7 @@
       </c>
       <c r="O115" s="21"/>
     </row>
-    <row r="116" spans="1:15" ht="120" hidden="1">
+    <row r="116" spans="1:15" ht="115.2" hidden="1">
       <c r="A116" s="14">
         <v>115</v>
       </c>
@@ -7177,7 +7179,7 @@
       </c>
       <c r="O116" s="21"/>
     </row>
-    <row r="117" spans="1:15" ht="120" hidden="1">
+    <row r="117" spans="1:15" ht="115.2" hidden="1">
       <c r="A117" s="14">
         <v>116</v>
       </c>
@@ -7206,7 +7208,7 @@
       </c>
       <c r="O117" s="21"/>
     </row>
-    <row r="118" spans="1:15" ht="120" hidden="1">
+    <row r="118" spans="1:15" ht="115.2" hidden="1">
       <c r="A118" s="14">
         <v>117</v>
       </c>
@@ -7235,7 +7237,7 @@
       </c>
       <c r="O118" s="21"/>
     </row>
-    <row r="119" spans="1:15" ht="120" hidden="1">
+    <row r="119" spans="1:15" ht="115.2" hidden="1">
       <c r="A119" s="14">
         <v>118</v>
       </c>
@@ -7264,7 +7266,7 @@
       </c>
       <c r="O119" s="21"/>
     </row>
-    <row r="120" spans="1:15" ht="120" hidden="1">
+    <row r="120" spans="1:15" ht="115.2" hidden="1">
       <c r="A120" s="14">
         <v>119</v>
       </c>
@@ -7293,7 +7295,7 @@
       </c>
       <c r="O120" s="21"/>
     </row>
-    <row r="121" spans="1:15" ht="120" hidden="1">
+    <row r="121" spans="1:15" ht="115.2" hidden="1">
       <c r="A121" s="14">
         <v>120</v>
       </c>
@@ -7322,7 +7324,7 @@
       </c>
       <c r="O121" s="21"/>
     </row>
-    <row r="122" spans="1:15" ht="120" hidden="1">
+    <row r="122" spans="1:15" ht="115.2" hidden="1">
       <c r="A122" s="14">
         <v>121</v>
       </c>
@@ -7351,7 +7353,7 @@
       </c>
       <c r="O122" s="21"/>
     </row>
-    <row r="123" spans="1:15" ht="105" hidden="1">
+    <row r="123" spans="1:15" ht="100.8" hidden="1">
       <c r="A123" s="14">
         <v>122</v>
       </c>
@@ -7380,7 +7382,7 @@
       </c>
       <c r="O123" s="21"/>
     </row>
-    <row r="124" spans="1:15" ht="105" hidden="1">
+    <row r="124" spans="1:15" ht="100.8" hidden="1">
       <c r="A124" s="14">
         <v>123</v>
       </c>
@@ -7409,7 +7411,7 @@
       </c>
       <c r="O124" s="21"/>
     </row>
-    <row r="125" spans="1:15" ht="105" hidden="1">
+    <row r="125" spans="1:15" ht="100.8" hidden="1">
       <c r="A125" s="14">
         <v>124</v>
       </c>
@@ -7438,7 +7440,7 @@
       </c>
       <c r="O125" s="21"/>
     </row>
-    <row r="126" spans="1:15" ht="120" hidden="1">
+    <row r="126" spans="1:15" ht="115.2" hidden="1">
       <c r="A126" s="14">
         <v>125</v>
       </c>
@@ -7467,7 +7469,7 @@
       </c>
       <c r="O126" s="21"/>
     </row>
-    <row r="127" spans="1:15" ht="105" hidden="1">
+    <row r="127" spans="1:15" ht="100.8" hidden="1">
       <c r="A127" s="14">
         <v>126</v>
       </c>
@@ -7496,7 +7498,7 @@
       </c>
       <c r="O127" s="21"/>
     </row>
-    <row r="128" spans="1:15" ht="105" hidden="1">
+    <row r="128" spans="1:15" ht="100.8" hidden="1">
       <c r="A128" s="14">
         <v>127</v>
       </c>
@@ -7525,7 +7527,7 @@
       </c>
       <c r="O128" s="21"/>
     </row>
-    <row r="129" spans="1:15" ht="105" hidden="1">
+    <row r="129" spans="1:15" ht="100.8" hidden="1">
       <c r="A129" s="14">
         <v>128</v>
       </c>
@@ -7554,7 +7556,7 @@
       </c>
       <c r="O129" s="21"/>
     </row>
-    <row r="130" spans="1:15" ht="120" hidden="1">
+    <row r="130" spans="1:15" ht="115.2" hidden="1">
       <c r="A130" s="14">
         <v>129</v>
       </c>
@@ -7583,7 +7585,7 @@
       </c>
       <c r="O130" s="21"/>
     </row>
-    <row r="131" spans="1:15" ht="105" hidden="1">
+    <row r="131" spans="1:15" ht="100.8" hidden="1">
       <c r="A131" s="14">
         <v>130</v>
       </c>
@@ -7612,7 +7614,7 @@
       </c>
       <c r="O131" s="21"/>
     </row>
-    <row r="132" spans="1:15" ht="105" hidden="1">
+    <row r="132" spans="1:15" ht="100.8" hidden="1">
       <c r="A132" s="14">
         <v>131</v>
       </c>
@@ -7641,7 +7643,7 @@
       </c>
       <c r="O132" s="21"/>
     </row>
-    <row r="133" spans="1:15" ht="105" hidden="1">
+    <row r="133" spans="1:15" ht="100.8" hidden="1">
       <c r="A133" s="14">
         <v>132</v>
       </c>
@@ -7670,7 +7672,7 @@
       </c>
       <c r="O133" s="21"/>
     </row>
-    <row r="134" spans="1:15" ht="120" hidden="1">
+    <row r="134" spans="1:15" ht="115.2" hidden="1">
       <c r="A134" s="14">
         <v>133</v>
       </c>
@@ -7699,7 +7701,7 @@
       </c>
       <c r="O134" s="21"/>
     </row>
-    <row r="135" spans="1:15" ht="105" hidden="1">
+    <row r="135" spans="1:15" ht="100.8" hidden="1">
       <c r="A135" s="14">
         <v>134</v>
       </c>
@@ -7728,7 +7730,7 @@
       </c>
       <c r="O135" s="21"/>
     </row>
-    <row r="136" spans="1:15" ht="105" hidden="1">
+    <row r="136" spans="1:15" ht="100.8" hidden="1">
       <c r="A136" s="14">
         <v>135</v>
       </c>
@@ -7757,7 +7759,7 @@
       </c>
       <c r="O136" s="21"/>
     </row>
-    <row r="137" spans="1:15" ht="105" hidden="1">
+    <row r="137" spans="1:15" ht="100.8" hidden="1">
       <c r="A137" s="14">
         <v>136</v>
       </c>
@@ -7786,7 +7788,7 @@
       </c>
       <c r="O137" s="21"/>
     </row>
-    <row r="138" spans="1:15" ht="120" hidden="1">
+    <row r="138" spans="1:15" ht="115.2" hidden="1">
       <c r="A138" s="14">
         <v>137</v>
       </c>
@@ -7815,7 +7817,7 @@
       </c>
       <c r="O138" s="21"/>
     </row>
-    <row r="139" spans="1:15" ht="105" hidden="1">
+    <row r="139" spans="1:15" ht="100.8" hidden="1">
       <c r="A139" s="14">
         <v>138</v>
       </c>
@@ -7844,7 +7846,7 @@
       </c>
       <c r="O139" s="21"/>
     </row>
-    <row r="140" spans="1:15" ht="105" hidden="1">
+    <row r="140" spans="1:15" ht="100.8" hidden="1">
       <c r="A140" s="14">
         <v>139</v>
       </c>
@@ -7873,7 +7875,7 @@
       </c>
       <c r="O140" s="21"/>
     </row>
-    <row r="141" spans="1:15" ht="105" hidden="1">
+    <row r="141" spans="1:15" ht="100.8" hidden="1">
       <c r="A141" s="14">
         <v>140</v>
       </c>
@@ -7902,7 +7904,7 @@
       </c>
       <c r="O141" s="21"/>
     </row>
-    <row r="142" spans="1:15" ht="120" hidden="1">
+    <row r="142" spans="1:15" ht="115.2" hidden="1">
       <c r="A142" s="14">
         <v>141</v>
       </c>
@@ -7931,7 +7933,7 @@
       </c>
       <c r="O142" s="21"/>
     </row>
-    <row r="143" spans="1:15" ht="105" hidden="1">
+    <row r="143" spans="1:15" ht="100.8" hidden="1">
       <c r="A143" s="14">
         <v>142</v>
       </c>
@@ -7960,7 +7962,7 @@
       </c>
       <c r="O143" s="21"/>
     </row>
-    <row r="144" spans="1:15" ht="105" hidden="1">
+    <row r="144" spans="1:15" ht="100.8" hidden="1">
       <c r="A144" s="14">
         <v>143</v>
       </c>
@@ -7989,7 +7991,7 @@
       </c>
       <c r="O144" s="21"/>
     </row>
-    <row r="145" spans="1:15" ht="105" hidden="1">
+    <row r="145" spans="1:15" ht="100.8" hidden="1">
       <c r="A145" s="14">
         <v>144</v>
       </c>
@@ -8018,7 +8020,7 @@
       </c>
       <c r="O145" s="21"/>
     </row>
-    <row r="146" spans="1:15" ht="120" hidden="1">
+    <row r="146" spans="1:15" ht="115.2" hidden="1">
       <c r="A146" s="14">
         <v>145</v>
       </c>
@@ -8047,7 +8049,7 @@
       </c>
       <c r="O146" s="21"/>
     </row>
-    <row r="147" spans="1:15" ht="120" hidden="1">
+    <row r="147" spans="1:15" ht="115.2" hidden="1">
       <c r="A147" s="14">
         <v>146</v>
       </c>
@@ -18267,13 +18269,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="58.42578125" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.44140625" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -19377,11 +19379,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -20419,15 +20421,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA9DE3DB3C6091468D1D4005047F3381" ma:contentTypeVersion="4" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="459c8a6a3a88bd262a2ff1f0ba7a9f11">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ae8219d-8505-4e64-b47a-e5e02bd99ff8" xmlns:ns3="b6c6c545-4433-4453-a388-ae81a1a09069" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd389b9c591f38f50631ea74e6d4f129" ns2:_="" ns3:_="">
     <xsd:import namespace="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
@@ -20592,15 +20585,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44D316A-03D1-4D0D-8C30-961F2644D409}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D083E07-CB22-4B29-AE20-400E2F1FBB78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20617,4 +20611,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44D316A-03D1-4D0D-8C30-961F2644D409}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>